<commit_message>
Include fields for multi-year bias correction.
</commit_message>
<xml_diff>
--- a/2. Profile Generator/ControlFile_ProfileGenerator.xlsx
+++ b/2. Profile Generator/ControlFile_ProfileGenerator.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="177">
   <si>
     <t>Country</t>
   </si>
@@ -426,19 +426,37 @@
     <t>ERA5DataFilePath_Inst</t>
   </si>
   <si>
-    <t>C:\Dev\model_supply_regions\GitHub\Inputs\ERA5_Inst</t>
-  </si>
-  <si>
-    <t>path to instantaneous ERA 5 data (u10, v10, u100, v100, t2m, z)</t>
+    <t>C:\Dev\model_supply_regions\GitHub\Inputs\ERA5_Inst\</t>
+  </si>
+  <si>
+    <t>path to folder carrying instantaneous ERA 5 data  (u10, v10, u100, v100, t2m, z) for all other weather years</t>
   </si>
   <si>
     <t>ERA5DataFilePath_Acc</t>
   </si>
   <si>
-    <t>C:\Dev\model_supply_regions\GitHub\Inputs\ERA5_Acc</t>
-  </si>
-  <si>
-    <t>path to accumulated ERA 5 data (ssrd)</t>
+    <t>C:\Dev\model_supply_regions\GitHub\Inputs\ERA5_Acc\</t>
+  </si>
+  <si>
+    <t>path to folder carrying accumulated ERA 5 data (ssrd) for all other weather years</t>
+  </si>
+  <si>
+    <t>ERA5Data_fityear</t>
+  </si>
+  <si>
+    <t>Include the year used as fit year for the bias-correction</t>
+  </si>
+  <si>
+    <t>ERA5Data_startyear</t>
+  </si>
+  <si>
+    <t>Include the start year</t>
+  </si>
+  <si>
+    <t>ERA5Data_endyear</t>
+  </si>
+  <si>
+    <t>Include the end year</t>
   </si>
   <si>
     <t>Input_MSR_Folder</t>
@@ -639,10 +657,10 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -946,7 +964,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -979,7 +997,7 @@
         <v>137</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5" customFormat="1" s="7">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="33" customFormat="1" s="7">
       <c r="A3" s="10" t="s">
         <v>138</v>
       </c>
@@ -990,125 +1008,158 @@
         <v>140</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="33" customFormat="1" s="7">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5" customFormat="1" s="7">
       <c r="A4" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="12">
+        <v>2000</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="C4" s="10" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5" customFormat="1" s="7">
+      <c r="A5" s="10" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="33" customFormat="1" s="7">
-      <c r="A5" s="10" t="s">
+      <c r="B5" s="12">
+        <v>2000</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="B5" s="11" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5" customFormat="1" s="7">
+      <c r="A6" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="B6" s="12">
+        <v>2004</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>146</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="33" customFormat="1" s="7">
-      <c r="A6" s="10" t="s">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="33" customFormat="1" s="7">
+      <c r="A7" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B7" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C7" s="10" t="s">
         <v>149</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="33" customFormat="1" s="7">
+      <c r="A8" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B8" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>154</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="10" t="s">
         <v>152</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="33" customFormat="1" s="7">
       <c r="A9" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="C9" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="B9" s="11" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+      <c r="A10" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="B10" s="13" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="46.5" customFormat="1" s="7">
-      <c r="A10" s="10" t="s">
+      <c r="C10" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="B10" s="11" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+      <c r="A11" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="B11" s="13" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="46.5" customFormat="1" s="7">
-      <c r="A11" s="10" t="s">
+      <c r="C11" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="33" customFormat="1" s="7">
+      <c r="A12" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B12" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C12" s="10" t="s">
         <v>163</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
-      <c r="A12" s="10" t="s">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="46.5" customFormat="1" s="7">
+      <c r="A13" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B13" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C13" s="10" t="s">
         <v>166</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
-      <c r="A13" s="10" t="s">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="33" customFormat="1" s="7">
+      <c r="A14" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B14" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="20.25">
-      <c r="A14" s="10" t="s">
+      <c r="C14" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="B14" s="13">
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+      <c r="A15" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+      <c r="A16" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="20.25">
+      <c r="A17" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B17" s="12">
         <v>720</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>170</v>
+      <c r="C17" s="3" t="s">
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -1159,7 +1210,7 @@
         <v>131</v>
       </c>
       <c r="B3" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>130</v>

</xml_diff>